<commit_message>
nmv 22 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TS 1.3" sheetId="1" r:id="rId1"/>
-    <sheet name="TS 1.4" sheetId="2" r:id="rId2"/>
-    <sheet name="TS 1.5" sheetId="3" r:id="rId3"/>
-    <sheet name="TS 1.6" sheetId="4" r:id="rId4"/>
-    <sheet name="TS 1.7" sheetId="5" r:id="rId5"/>
-    <sheet name="TS 1.8" sheetId="6" r:id="rId6"/>
-    <sheet name="total 1 to 8" sheetId="7" r:id="rId7"/>
+    <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
+    <sheet name="TS 1.2" sheetId="9" r:id="rId2"/>
+    <sheet name="TS 1.3" sheetId="1" r:id="rId3"/>
+    <sheet name="TS 1.4" sheetId="2" r:id="rId4"/>
+    <sheet name="TS 1.5" sheetId="3" r:id="rId5"/>
+    <sheet name="TS 1.6" sheetId="4" r:id="rId6"/>
+    <sheet name="TS 1.7" sheetId="5" r:id="rId7"/>
+    <sheet name="TS 1.8" sheetId="6" r:id="rId8"/>
+    <sheet name="total 1 to 8" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="355">
   <si>
     <t>1.3.1.1 :</t>
   </si>
@@ -2118,12 +2120,96 @@
   <si>
     <t>Prasnam No.1 to 8</t>
   </si>
+  <si>
+    <t>1.1.1.1 :</t>
+  </si>
+  <si>
+    <t>1.1.2.1 :</t>
+  </si>
+  <si>
+    <t>1.1.2.2 :</t>
+  </si>
+  <si>
+    <t>1.1.3.1 :</t>
+  </si>
+  <si>
+    <t>1.1.4.1 :</t>
+  </si>
+  <si>
+    <t>1.1.4.2 :</t>
+  </si>
+  <si>
+    <t>1.1.5.1 :</t>
+  </si>
+  <si>
+    <t>1.1.5.2 :</t>
+  </si>
+  <si>
+    <t>1.1.6.1 :</t>
+  </si>
+  <si>
+    <t>1.1.7.1 :</t>
+  </si>
+  <si>
+    <t>1.1.7.2 :</t>
+  </si>
+  <si>
+    <t>1.1.8.1 :</t>
+  </si>
+  <si>
+    <t>1.1.9.1 :</t>
+  </si>
+  <si>
+    <t>1.1.9.2 :</t>
+  </si>
+  <si>
+    <t>1.1.9.3 :</t>
+  </si>
+  <si>
+    <t>1.1.10.1 :</t>
+  </si>
+  <si>
+    <t>1.1.10.2 :</t>
+  </si>
+  <si>
+    <t>1.1.10.3 :</t>
+  </si>
+  <si>
+    <t>1.1.11.1 :</t>
+  </si>
+  <si>
+    <t>1.1.11.2 :</t>
+  </si>
+  <si>
+    <t>1.1.12.1 :</t>
+  </si>
+  <si>
+    <t>1.1.13.1 :</t>
+  </si>
+  <si>
+    <t>1.1.13.2 :</t>
+  </si>
+  <si>
+    <t>1.1.13.3 :</t>
+  </si>
+  <si>
+    <t>1.1.14.1 :</t>
+  </si>
+  <si>
+    <t>1.1.14.2 :</t>
+  </si>
+  <si>
+    <t>1.1.14.3 :</t>
+  </si>
+  <si>
+    <t>1.1.14.4 :</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2200,8 +2286,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2232,8 +2325,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2323,11 +2422,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2437,6 +2588,33 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2719,6 +2897,1291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" s="40">
+        <v>6</v>
+      </c>
+      <c r="C3" s="40">
+        <v>0</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0</v>
+      </c>
+      <c r="E3" s="40">
+        <v>0</v>
+      </c>
+      <c r="F3" s="40">
+        <v>1</v>
+      </c>
+      <c r="G3" s="40">
+        <v>3</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0</v>
+      </c>
+      <c r="I3" s="40">
+        <v>0</v>
+      </c>
+      <c r="J3" s="40">
+        <v>36</v>
+      </c>
+      <c r="K3" s="40">
+        <v>43</v>
+      </c>
+      <c r="L3" s="40">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="41" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" s="42">
+        <v>12</v>
+      </c>
+      <c r="C4" s="42">
+        <v>0</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42">
+        <v>0</v>
+      </c>
+      <c r="F4" s="42">
+        <v>0</v>
+      </c>
+      <c r="G4" s="42">
+        <v>2</v>
+      </c>
+      <c r="H4" s="42">
+        <v>0</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0</v>
+      </c>
+      <c r="J4" s="42">
+        <v>38</v>
+      </c>
+      <c r="K4" s="42">
+        <v>50</v>
+      </c>
+      <c r="L4" s="42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
+        <v>329</v>
+      </c>
+      <c r="B5" s="42">
+        <v>5</v>
+      </c>
+      <c r="C5" s="42">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42">
+        <v>0</v>
+      </c>
+      <c r="E5" s="42">
+        <v>0</v>
+      </c>
+      <c r="F5" s="42">
+        <v>1</v>
+      </c>
+      <c r="G5" s="42">
+        <v>4</v>
+      </c>
+      <c r="H5" s="42">
+        <v>0</v>
+      </c>
+      <c r="I5" s="42">
+        <v>0</v>
+      </c>
+      <c r="J5" s="42">
+        <v>32</v>
+      </c>
+      <c r="K5" s="42">
+        <v>38</v>
+      </c>
+      <c r="L5" s="42">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="42">
+        <v>10</v>
+      </c>
+      <c r="C6" s="42">
+        <v>0</v>
+      </c>
+      <c r="D6" s="42">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42">
+        <v>0</v>
+      </c>
+      <c r="F6" s="42">
+        <v>1</v>
+      </c>
+      <c r="G6" s="42">
+        <v>2</v>
+      </c>
+      <c r="H6" s="42">
+        <v>0</v>
+      </c>
+      <c r="I6" s="42">
+        <v>0</v>
+      </c>
+      <c r="J6" s="42">
+        <v>46</v>
+      </c>
+      <c r="K6" s="42">
+        <v>58</v>
+      </c>
+      <c r="L6" s="42">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" s="42">
+        <v>8</v>
+      </c>
+      <c r="C7" s="42">
+        <v>0</v>
+      </c>
+      <c r="D7" s="42">
+        <v>0</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+      <c r="F7" s="42">
+        <v>0</v>
+      </c>
+      <c r="G7" s="42">
+        <v>2</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0</v>
+      </c>
+      <c r="J7" s="42">
+        <v>42</v>
+      </c>
+      <c r="K7" s="42">
+        <v>50</v>
+      </c>
+      <c r="L7" s="42">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="42">
+        <v>5</v>
+      </c>
+      <c r="C8" s="42">
+        <v>0</v>
+      </c>
+      <c r="D8" s="42">
+        <v>0</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0</v>
+      </c>
+      <c r="F8" s="42">
+        <v>1</v>
+      </c>
+      <c r="G8" s="42">
+        <v>4</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0</v>
+      </c>
+      <c r="I8" s="42">
+        <v>0</v>
+      </c>
+      <c r="J8" s="42">
+        <v>40</v>
+      </c>
+      <c r="K8" s="42">
+        <v>46</v>
+      </c>
+      <c r="L8" s="42">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="B9" s="42">
+        <v>11</v>
+      </c>
+      <c r="C9" s="42">
+        <v>0</v>
+      </c>
+      <c r="D9" s="42">
+        <v>0</v>
+      </c>
+      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+      <c r="F9" s="42">
+        <v>0</v>
+      </c>
+      <c r="G9" s="42">
+        <v>3</v>
+      </c>
+      <c r="H9" s="42">
+        <v>0</v>
+      </c>
+      <c r="I9" s="42">
+        <v>0</v>
+      </c>
+      <c r="J9" s="42">
+        <v>39</v>
+      </c>
+      <c r="K9" s="42">
+        <v>50</v>
+      </c>
+      <c r="L9" s="42">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
+        <v>334</v>
+      </c>
+      <c r="B10" s="42">
+        <v>11</v>
+      </c>
+      <c r="C10" s="42">
+        <v>0</v>
+      </c>
+      <c r="D10" s="42">
+        <v>0</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0</v>
+      </c>
+      <c r="F10" s="42">
+        <v>1</v>
+      </c>
+      <c r="G10" s="42">
+        <v>6</v>
+      </c>
+      <c r="H10" s="42">
+        <v>0</v>
+      </c>
+      <c r="I10" s="42">
+        <v>0</v>
+      </c>
+      <c r="J10" s="42">
+        <v>49</v>
+      </c>
+      <c r="K10" s="42">
+        <v>61</v>
+      </c>
+      <c r="L10" s="42">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="42">
+        <v>9</v>
+      </c>
+      <c r="C11" s="42">
+        <v>0</v>
+      </c>
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="F11" s="42">
+        <v>1</v>
+      </c>
+      <c r="G11" s="42">
+        <v>7</v>
+      </c>
+      <c r="H11" s="42">
+        <v>0</v>
+      </c>
+      <c r="I11" s="42">
+        <v>0</v>
+      </c>
+      <c r="J11" s="42">
+        <v>55</v>
+      </c>
+      <c r="K11" s="42">
+        <v>65</v>
+      </c>
+      <c r="L11" s="42">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" s="42">
+        <v>10</v>
+      </c>
+      <c r="C12" s="42">
+        <v>0</v>
+      </c>
+      <c r="D12" s="42">
+        <v>0</v>
+      </c>
+      <c r="E12" s="42">
+        <v>0</v>
+      </c>
+      <c r="F12" s="42">
+        <v>0</v>
+      </c>
+      <c r="G12" s="42">
+        <v>5</v>
+      </c>
+      <c r="H12" s="42">
+        <v>0</v>
+      </c>
+      <c r="I12" s="42">
+        <v>0</v>
+      </c>
+      <c r="J12" s="42">
+        <v>40</v>
+      </c>
+      <c r="K12" s="42">
+        <v>50</v>
+      </c>
+      <c r="L12" s="42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="42">
+        <v>6</v>
+      </c>
+      <c r="C13" s="42">
+        <v>0</v>
+      </c>
+      <c r="D13" s="42">
+        <v>1</v>
+      </c>
+      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="F13" s="42">
+        <v>2</v>
+      </c>
+      <c r="G13" s="42">
+        <v>5</v>
+      </c>
+      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="I13" s="42">
+        <v>0</v>
+      </c>
+      <c r="J13" s="42">
+        <v>39</v>
+      </c>
+      <c r="K13" s="42">
+        <v>48</v>
+      </c>
+      <c r="L13" s="42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>338</v>
+      </c>
+      <c r="B14" s="42">
+        <v>11</v>
+      </c>
+      <c r="C14" s="42">
+        <v>0</v>
+      </c>
+      <c r="D14" s="42">
+        <v>0</v>
+      </c>
+      <c r="E14" s="42">
+        <v>0</v>
+      </c>
+      <c r="F14" s="42">
+        <v>1</v>
+      </c>
+      <c r="G14" s="42">
+        <v>10</v>
+      </c>
+      <c r="H14" s="42">
+        <v>0</v>
+      </c>
+      <c r="I14" s="42">
+        <v>0</v>
+      </c>
+      <c r="J14" s="42">
+        <v>60</v>
+      </c>
+      <c r="K14" s="42">
+        <v>72</v>
+      </c>
+      <c r="L14" s="42">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="B15" s="42">
+        <v>9</v>
+      </c>
+      <c r="C15" s="42">
+        <v>0</v>
+      </c>
+      <c r="D15" s="42">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42">
+        <v>0</v>
+      </c>
+      <c r="G15" s="42">
+        <v>1</v>
+      </c>
+      <c r="H15" s="42">
+        <v>0</v>
+      </c>
+      <c r="I15" s="42">
+        <v>0</v>
+      </c>
+      <c r="J15" s="42">
+        <v>41</v>
+      </c>
+      <c r="K15" s="42">
+        <v>50</v>
+      </c>
+      <c r="L15" s="42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" s="42">
+        <v>6</v>
+      </c>
+      <c r="C16" s="42">
+        <v>0</v>
+      </c>
+      <c r="D16" s="42">
+        <v>0</v>
+      </c>
+      <c r="E16" s="42">
+        <v>0</v>
+      </c>
+      <c r="F16" s="42">
+        <v>0</v>
+      </c>
+      <c r="G16" s="42">
+        <v>0</v>
+      </c>
+      <c r="H16" s="42">
+        <v>0</v>
+      </c>
+      <c r="I16" s="42">
+        <v>0</v>
+      </c>
+      <c r="J16" s="42">
+        <v>44</v>
+      </c>
+      <c r="K16" s="42">
+        <v>50</v>
+      </c>
+      <c r="L16" s="42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="B17" s="42">
+        <v>9</v>
+      </c>
+      <c r="C17" s="42">
+        <v>0</v>
+      </c>
+      <c r="D17" s="42">
+        <v>0</v>
+      </c>
+      <c r="E17" s="42">
+        <v>0</v>
+      </c>
+      <c r="F17" s="42">
+        <v>1</v>
+      </c>
+      <c r="G17" s="42">
+        <v>3</v>
+      </c>
+      <c r="H17" s="42">
+        <v>0</v>
+      </c>
+      <c r="I17" s="42">
+        <v>0</v>
+      </c>
+      <c r="J17" s="42">
+        <v>51</v>
+      </c>
+      <c r="K17" s="42">
+        <v>61</v>
+      </c>
+      <c r="L17" s="42">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="B18" s="42">
+        <v>13</v>
+      </c>
+      <c r="C18" s="42">
+        <v>0</v>
+      </c>
+      <c r="D18" s="42">
+        <v>0</v>
+      </c>
+      <c r="E18" s="42">
+        <v>0</v>
+      </c>
+      <c r="F18" s="42">
+        <v>2</v>
+      </c>
+      <c r="G18" s="42">
+        <v>7</v>
+      </c>
+      <c r="H18" s="42">
+        <v>0</v>
+      </c>
+      <c r="I18" s="42">
+        <v>0</v>
+      </c>
+      <c r="J18" s="42">
+        <v>35</v>
+      </c>
+      <c r="K18" s="42">
+        <v>50</v>
+      </c>
+      <c r="L18" s="42">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="B19" s="42">
+        <v>4</v>
+      </c>
+      <c r="C19" s="42">
+        <v>1</v>
+      </c>
+      <c r="D19" s="42">
+        <v>0</v>
+      </c>
+      <c r="E19" s="42">
+        <v>0</v>
+      </c>
+      <c r="F19" s="42">
+        <v>6</v>
+      </c>
+      <c r="G19" s="42">
+        <v>6</v>
+      </c>
+      <c r="H19" s="42">
+        <v>0</v>
+      </c>
+      <c r="I19" s="42">
+        <v>0</v>
+      </c>
+      <c r="J19" s="42">
+        <v>41</v>
+      </c>
+      <c r="K19" s="42">
+        <v>50</v>
+      </c>
+      <c r="L19" s="42">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" s="42">
+        <v>9</v>
+      </c>
+      <c r="C20" s="42">
+        <v>0</v>
+      </c>
+      <c r="D20" s="42">
+        <v>0</v>
+      </c>
+      <c r="E20" s="42">
+        <v>0</v>
+      </c>
+      <c r="F20" s="42">
+        <v>1</v>
+      </c>
+      <c r="G20" s="46">
+        <v>5</v>
+      </c>
+      <c r="H20" s="42">
+        <v>0</v>
+      </c>
+      <c r="I20" s="42">
+        <v>0</v>
+      </c>
+      <c r="J20" s="42">
+        <v>56</v>
+      </c>
+      <c r="K20" s="42">
+        <v>66</v>
+      </c>
+      <c r="L20" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="B21" s="42">
+        <v>9</v>
+      </c>
+      <c r="C21" s="42">
+        <v>0</v>
+      </c>
+      <c r="D21" s="42">
+        <v>0</v>
+      </c>
+      <c r="E21" s="42">
+        <v>0</v>
+      </c>
+      <c r="F21" s="42">
+        <v>0</v>
+      </c>
+      <c r="G21" s="42">
+        <v>0</v>
+      </c>
+      <c r="H21" s="42">
+        <v>0</v>
+      </c>
+      <c r="I21" s="42">
+        <v>0</v>
+      </c>
+      <c r="J21" s="42">
+        <v>41</v>
+      </c>
+      <c r="K21" s="42">
+        <v>50</v>
+      </c>
+      <c r="L21" s="42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="B22" s="42">
+        <v>11</v>
+      </c>
+      <c r="C22" s="42">
+        <v>1</v>
+      </c>
+      <c r="D22" s="42">
+        <v>2</v>
+      </c>
+      <c r="E22" s="42">
+        <v>0</v>
+      </c>
+      <c r="F22" s="42">
+        <v>1</v>
+      </c>
+      <c r="G22" s="42">
+        <v>2</v>
+      </c>
+      <c r="H22" s="42">
+        <v>0</v>
+      </c>
+      <c r="I22" s="42">
+        <v>0</v>
+      </c>
+      <c r="J22" s="42">
+        <v>52</v>
+      </c>
+      <c r="K22" s="42">
+        <v>65</v>
+      </c>
+      <c r="L22" s="42">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="B23" s="42">
+        <v>10</v>
+      </c>
+      <c r="C23" s="42">
+        <v>0</v>
+      </c>
+      <c r="D23" s="42">
+        <v>1</v>
+      </c>
+      <c r="E23" s="42">
+        <v>0</v>
+      </c>
+      <c r="F23" s="42">
+        <v>2</v>
+      </c>
+      <c r="G23" s="42">
+        <v>7</v>
+      </c>
+      <c r="H23" s="42">
+        <v>0</v>
+      </c>
+      <c r="I23" s="42">
+        <v>0</v>
+      </c>
+      <c r="J23" s="42">
+        <v>58</v>
+      </c>
+      <c r="K23" s="42">
+        <v>71</v>
+      </c>
+      <c r="L23" s="42">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="B24" s="42">
+        <v>7</v>
+      </c>
+      <c r="C24" s="42">
+        <v>0</v>
+      </c>
+      <c r="D24" s="42">
+        <v>1</v>
+      </c>
+      <c r="E24" s="42">
+        <v>0</v>
+      </c>
+      <c r="F24" s="42">
+        <v>5</v>
+      </c>
+      <c r="G24" s="42">
+        <v>4</v>
+      </c>
+      <c r="H24" s="42">
+        <v>0</v>
+      </c>
+      <c r="I24" s="42">
+        <v>2</v>
+      </c>
+      <c r="J24" s="42">
+        <v>37</v>
+      </c>
+      <c r="K24" s="42">
+        <v>50</v>
+      </c>
+      <c r="L24" s="42">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="B25" s="42">
+        <v>9</v>
+      </c>
+      <c r="C25" s="42">
+        <v>0</v>
+      </c>
+      <c r="D25" s="42">
+        <v>0</v>
+      </c>
+      <c r="E25" s="42">
+        <v>0</v>
+      </c>
+      <c r="F25" s="42">
+        <v>2</v>
+      </c>
+      <c r="G25" s="47">
+        <v>4</v>
+      </c>
+      <c r="H25" s="42">
+        <v>0</v>
+      </c>
+      <c r="I25" s="42">
+        <v>0</v>
+      </c>
+      <c r="J25" s="42">
+        <v>39</v>
+      </c>
+      <c r="K25" s="42">
+        <v>50</v>
+      </c>
+      <c r="L25" s="42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="41" t="s">
+        <v>350</v>
+      </c>
+      <c r="B26" s="42">
+        <v>8</v>
+      </c>
+      <c r="C26" s="42">
+        <v>0</v>
+      </c>
+      <c r="D26" s="42">
+        <v>3</v>
+      </c>
+      <c r="E26" s="42">
+        <v>0</v>
+      </c>
+      <c r="F26" s="42">
+        <v>1</v>
+      </c>
+      <c r="G26" s="42">
+        <v>1</v>
+      </c>
+      <c r="H26" s="42">
+        <v>0</v>
+      </c>
+      <c r="I26" s="42">
+        <v>0</v>
+      </c>
+      <c r="J26" s="42">
+        <v>51</v>
+      </c>
+      <c r="K26" s="42">
+        <v>63</v>
+      </c>
+      <c r="L26" s="42">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="41" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" s="42">
+        <v>7</v>
+      </c>
+      <c r="C27" s="42">
+        <v>0</v>
+      </c>
+      <c r="D27" s="42">
+        <v>4</v>
+      </c>
+      <c r="E27" s="42">
+        <v>0</v>
+      </c>
+      <c r="F27" s="42">
+        <v>7</v>
+      </c>
+      <c r="G27" s="42">
+        <v>0</v>
+      </c>
+      <c r="H27" s="42">
+        <v>0</v>
+      </c>
+      <c r="I27" s="42">
+        <v>2</v>
+      </c>
+      <c r="J27" s="42">
+        <v>32</v>
+      </c>
+      <c r="K27" s="42">
+        <v>50</v>
+      </c>
+      <c r="L27" s="42">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="41" t="s">
+        <v>352</v>
+      </c>
+      <c r="B28" s="42">
+        <v>6</v>
+      </c>
+      <c r="C28" s="42">
+        <v>1</v>
+      </c>
+      <c r="D28" s="42">
+        <v>0</v>
+      </c>
+      <c r="E28" s="42">
+        <v>0</v>
+      </c>
+      <c r="F28" s="42">
+        <v>6</v>
+      </c>
+      <c r="G28" s="42">
+        <v>3</v>
+      </c>
+      <c r="H28" s="42">
+        <v>0</v>
+      </c>
+      <c r="I28" s="42">
+        <v>0</v>
+      </c>
+      <c r="J28" s="42">
+        <v>39</v>
+      </c>
+      <c r="K28" s="42">
+        <v>50</v>
+      </c>
+      <c r="L28" s="42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="41" t="s">
+        <v>353</v>
+      </c>
+      <c r="B29" s="42">
+        <v>6</v>
+      </c>
+      <c r="C29" s="42">
+        <v>1</v>
+      </c>
+      <c r="D29" s="42">
+        <v>0</v>
+      </c>
+      <c r="E29" s="42">
+        <v>0</v>
+      </c>
+      <c r="F29" s="42">
+        <v>6</v>
+      </c>
+      <c r="G29" s="42">
+        <v>3</v>
+      </c>
+      <c r="H29" s="42">
+        <v>0</v>
+      </c>
+      <c r="I29" s="42">
+        <v>0</v>
+      </c>
+      <c r="J29" s="42">
+        <v>39</v>
+      </c>
+      <c r="K29" s="42">
+        <v>50</v>
+      </c>
+      <c r="L29" s="42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="41" t="s">
+        <v>354</v>
+      </c>
+      <c r="B30" s="42">
+        <v>7</v>
+      </c>
+      <c r="C30" s="42">
+        <v>2</v>
+      </c>
+      <c r="D30" s="42">
+        <v>0</v>
+      </c>
+      <c r="E30" s="42">
+        <v>0</v>
+      </c>
+      <c r="F30" s="42">
+        <v>9</v>
+      </c>
+      <c r="G30" s="42">
+        <v>5</v>
+      </c>
+      <c r="H30" s="42">
+        <v>1</v>
+      </c>
+      <c r="I30" s="42">
+        <v>2</v>
+      </c>
+      <c r="J30" s="42">
+        <v>59</v>
+      </c>
+      <c r="K30" s="42">
+        <v>73</v>
+      </c>
+      <c r="L30" s="42">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="43">
+        <v>28</v>
+      </c>
+      <c r="B31" s="44">
+        <f>SUM(B3:B30)</f>
+        <v>234</v>
+      </c>
+      <c r="C31" s="44">
+        <f t="shared" ref="C31:L31" si="0">SUM(C3:C30)</f>
+        <v>6</v>
+      </c>
+      <c r="D31" s="44">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="44">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="G31" s="44">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="H31" s="44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I31" s="44">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J31" s="44">
+        <f t="shared" si="0"/>
+        <v>1231</v>
+      </c>
+      <c r="K31" s="44">
+        <f t="shared" si="0"/>
+        <v>1530</v>
+      </c>
+      <c r="L31" s="44">
+        <f t="shared" si="0"/>
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="45"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32">
+        <f>G31</f>
+        <v>104</v>
+      </c>
+      <c r="J32">
+        <f>B31-C31</f>
+        <v>228</v>
+      </c>
+      <c r="K32" s="22"/>
+      <c r="L32" s="45"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33">
+        <f>B31</f>
+        <v>234</v>
+      </c>
+      <c r="J33">
+        <f>D31-E31</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <f>K31</f>
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f>SUM(F32:F36)</f>
+        <v>351</v>
+      </c>
+      <c r="J37">
+        <f>SUM(J32:J36)</f>
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f>K31-F37</f>
+        <v>1179</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39">
+        <f>J37-L31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f>F37+F38</f>
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f>F40-K31</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4089,7 +5552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
@@ -6356,7 +7819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
@@ -8511,7 +9974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
@@ -10676,7 +12139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
@@ -12830,13 +14293,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45:K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14648,7 +16111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M9"/>
   <sheetViews>

</xml_diff>

<commit_message>
nmv 23 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
@@ -4323,7 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -5833,9 +5833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6216,7 +6216,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -7052,7 +7052,7 @@
         <v>12</v>
       </c>
       <c r="G32" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
@@ -7096,7 +7096,7 @@
       </c>
       <c r="G33" s="6">
         <f t="shared" si="0"/>
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
@@ -7129,7 +7129,7 @@
       </c>
       <c r="F36">
         <f>G33</f>
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J36">
         <f>B33-C33</f>
@@ -7175,13 +7175,13 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F41">
         <f>SUM(F36:F40)</f>
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F42">
         <f>K33-F41</f>
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nmv 24 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
@@ -5833,8 +5833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -7205,9 +7205,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59:J69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8916,7 +8916,7 @@
         <v>6</v>
       </c>
       <c r="G45" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H45" s="11">
         <v>0</v>
@@ -9144,7 +9144,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H51" s="11">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>6</v>
       </c>
       <c r="G53" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H53" s="11">
         <v>0</v>
@@ -9296,7 +9296,7 @@
         <v>11</v>
       </c>
       <c r="G55" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H55" s="11">
         <v>0</v>
@@ -9340,7 +9340,7 @@
       </c>
       <c r="G56" s="13">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H56" s="13">
         <f t="shared" si="0"/>
@@ -9369,7 +9369,7 @@
       </c>
       <c r="F59">
         <f>G56</f>
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J59">
         <f>B56-C56</f>
@@ -9420,7 +9420,7 @@
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F64">
         <f>SUM(F59:F63)</f>
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="J64">
         <f>SUM(J59:J63)</f>
@@ -9430,7 +9430,7 @@
     <row r="65" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F65">
         <f>K56-F64</f>
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
nmv 25 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
@@ -7205,7 +7205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
@@ -9472,9 +9472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54:J64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9551,7 +9551,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="11">
         <v>0</v>
@@ -9627,7 +9627,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H4" s="11">
         <v>0</v>
@@ -9855,7 +9855,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="11">
         <v>0</v>
@@ -9969,7 +9969,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="11">
         <v>0</v>
@@ -10729,7 +10729,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H33" s="11">
         <v>0</v>
@@ -11147,7 +11147,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H44" s="11">
         <v>0</v>
@@ -11261,7 +11261,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H47" s="11">
         <v>0</v>
@@ -11299,7 +11299,7 @@
         <v>7</v>
       </c>
       <c r="G48" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H48" s="11">
         <v>0</v>
@@ -11451,7 +11451,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H52" s="11">
         <v>0</v>
@@ -11495,7 +11495,7 @@
       </c>
       <c r="G53" s="16">
         <f t="shared" si="0"/>
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="H53" s="16">
         <f t="shared" si="0"/>
@@ -11524,7 +11524,7 @@
       </c>
       <c r="F54">
         <f>G53</f>
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="J54">
         <f>B53-C53</f>
@@ -11575,7 +11575,7 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F59">
         <f>SUM(F54:F58)</f>
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="J59">
         <f>SUM(J54:J58)</f>
@@ -11585,7 +11585,7 @@
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F60">
         <f>K53-F59</f>
-        <v>2139</v>
+        <v>2129</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
nmv 26 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
@@ -2765,10 +2765,10 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4333,14 +4333,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="48"/>
@@ -11630,7 +11630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L53"/>
     </sheetView>
@@ -11707,7 +11707,7 @@
       <c r="F2" s="11">
         <v>3</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="55">
         <v>1</v>
       </c>
       <c r="H2" s="11">
@@ -11745,7 +11745,7 @@
       <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="56">
+      <c r="G3" s="55">
         <v>1</v>
       </c>
       <c r="H3" s="11">
@@ -11783,7 +11783,7 @@
       <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="55">
         <v>0</v>
       </c>
       <c r="H4" s="11">
@@ -11821,7 +11821,7 @@
       <c r="F5" s="11">
         <v>2</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="55">
         <v>0</v>
       </c>
       <c r="H5" s="11">
@@ -11859,7 +11859,7 @@
       <c r="F6" s="11">
         <v>3</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="55">
         <v>3</v>
       </c>
       <c r="H6" s="11">
@@ -11897,7 +11897,7 @@
       <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7" s="56">
+      <c r="G7" s="55">
         <v>1</v>
       </c>
       <c r="H7" s="11">
@@ -11935,7 +11935,7 @@
       <c r="F8" s="11">
         <v>1</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="55">
         <v>0</v>
       </c>
       <c r="H8" s="11">
@@ -11973,7 +11973,7 @@
       <c r="F9" s="11">
         <v>0</v>
       </c>
-      <c r="G9" s="56">
+      <c r="G9" s="55">
         <v>7</v>
       </c>
       <c r="H9" s="11">
@@ -12011,7 +12011,7 @@
       <c r="F10" s="11">
         <v>0</v>
       </c>
-      <c r="G10" s="56">
+      <c r="G10" s="55">
         <v>1</v>
       </c>
       <c r="H10" s="11">
@@ -12049,7 +12049,7 @@
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="56">
+      <c r="G11" s="55">
         <v>2</v>
       </c>
       <c r="H11" s="11">
@@ -12087,7 +12087,7 @@
       <c r="F12" s="11">
         <v>0</v>
       </c>
-      <c r="G12" s="56">
+      <c r="G12" s="55">
         <v>10</v>
       </c>
       <c r="H12" s="11">
@@ -12125,7 +12125,7 @@
       <c r="F13" s="11">
         <v>4</v>
       </c>
-      <c r="G13" s="56">
+      <c r="G13" s="55">
         <v>9</v>
       </c>
       <c r="H13" s="11">
@@ -12163,7 +12163,7 @@
       <c r="F14" s="11">
         <v>2</v>
       </c>
-      <c r="G14" s="56">
+      <c r="G14" s="55">
         <v>4</v>
       </c>
       <c r="H14" s="11">
@@ -12201,7 +12201,7 @@
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="56">
+      <c r="G15" s="55">
         <v>1</v>
       </c>
       <c r="H15" s="11">
@@ -12239,7 +12239,7 @@
       <c r="F16" s="11">
         <v>2</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="55">
         <v>2</v>
       </c>
       <c r="H16" s="11">
@@ -12277,7 +12277,7 @@
       <c r="F17" s="11">
         <v>1</v>
       </c>
-      <c r="G17" s="56">
+      <c r="G17" s="55">
         <v>8</v>
       </c>
       <c r="H17" s="11">
@@ -12315,7 +12315,7 @@
       <c r="F18" s="11">
         <v>1</v>
       </c>
-      <c r="G18" s="56">
+      <c r="G18" s="55">
         <v>2</v>
       </c>
       <c r="H18" s="11">
@@ -12353,7 +12353,7 @@
       <c r="F19" s="11">
         <v>3</v>
       </c>
-      <c r="G19" s="56">
+      <c r="G19" s="55">
         <v>6</v>
       </c>
       <c r="H19" s="11">
@@ -12391,7 +12391,7 @@
       <c r="F20" s="11">
         <v>1</v>
       </c>
-      <c r="G20" s="56">
+      <c r="G20" s="55">
         <v>4</v>
       </c>
       <c r="H20" s="11">
@@ -12429,7 +12429,7 @@
       <c r="F21" s="11">
         <v>4</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="55">
         <v>1</v>
       </c>
       <c r="H21" s="11">
@@ -12467,7 +12467,7 @@
       <c r="F22" s="11">
         <v>0</v>
       </c>
-      <c r="G22" s="56">
+      <c r="G22" s="55">
         <v>1</v>
       </c>
       <c r="H22" s="11">
@@ -12505,7 +12505,7 @@
       <c r="F23" s="11">
         <v>0</v>
       </c>
-      <c r="G23" s="56">
+      <c r="G23" s="55">
         <v>2</v>
       </c>
       <c r="H23" s="11">
@@ -12543,7 +12543,7 @@
       <c r="F24" s="11">
         <v>0</v>
       </c>
-      <c r="G24" s="56">
+      <c r="G24" s="55">
         <v>2</v>
       </c>
       <c r="H24" s="11">
@@ -12581,7 +12581,7 @@
       <c r="F25" s="11">
         <v>1</v>
       </c>
-      <c r="G25" s="56">
+      <c r="G25" s="55">
         <v>2</v>
       </c>
       <c r="H25" s="11">
@@ -12619,7 +12619,7 @@
       <c r="F26" s="11">
         <v>0</v>
       </c>
-      <c r="G26" s="56">
+      <c r="G26" s="55">
         <v>5</v>
       </c>
       <c r="H26" s="11">
@@ -12657,7 +12657,7 @@
       <c r="F27" s="11">
         <v>0</v>
       </c>
-      <c r="G27" s="56">
+      <c r="G27" s="55">
         <v>4</v>
       </c>
       <c r="H27" s="11">
@@ -12695,7 +12695,7 @@
       <c r="F28" s="11">
         <v>0</v>
       </c>
-      <c r="G28" s="56">
+      <c r="G28" s="55">
         <v>1</v>
       </c>
       <c r="H28" s="11">
@@ -12733,7 +12733,7 @@
       <c r="F29" s="11">
         <v>1</v>
       </c>
-      <c r="G29" s="56">
+      <c r="G29" s="55">
         <v>0</v>
       </c>
       <c r="H29" s="11">
@@ -12771,7 +12771,7 @@
       <c r="F30" s="11">
         <v>0</v>
       </c>
-      <c r="G30" s="56">
+      <c r="G30" s="55">
         <v>2</v>
       </c>
       <c r="H30" s="11">
@@ -12809,7 +12809,7 @@
       <c r="F31" s="11">
         <v>0</v>
       </c>
-      <c r="G31" s="56">
+      <c r="G31" s="55">
         <v>2</v>
       </c>
       <c r="H31" s="11">
@@ -12847,7 +12847,7 @@
       <c r="F32" s="11">
         <v>0</v>
       </c>
-      <c r="G32" s="56">
+      <c r="G32" s="55">
         <v>5</v>
       </c>
       <c r="H32" s="11">
@@ -12885,7 +12885,7 @@
       <c r="F33" s="11">
         <v>1</v>
       </c>
-      <c r="G33" s="56">
+      <c r="G33" s="55">
         <v>3</v>
       </c>
       <c r="H33" s="11">
@@ -12923,7 +12923,7 @@
       <c r="F34" s="11">
         <v>0</v>
       </c>
-      <c r="G34" s="56">
+      <c r="G34" s="55">
         <v>1</v>
       </c>
       <c r="H34" s="11">
@@ -12961,7 +12961,7 @@
       <c r="F35" s="11">
         <v>0</v>
       </c>
-      <c r="G35" s="56">
+      <c r="G35" s="55">
         <v>3</v>
       </c>
       <c r="H35" s="11">
@@ -12999,7 +12999,7 @@
       <c r="F36" s="11">
         <v>0</v>
       </c>
-      <c r="G36" s="56">
+      <c r="G36" s="55">
         <v>5</v>
       </c>
       <c r="H36" s="11">
@@ -13037,7 +13037,7 @@
       <c r="F37" s="11">
         <v>0</v>
       </c>
-      <c r="G37" s="56">
+      <c r="G37" s="55">
         <v>0</v>
       </c>
       <c r="H37" s="11">
@@ -13075,7 +13075,7 @@
       <c r="F38" s="11">
         <v>0</v>
       </c>
-      <c r="G38" s="56">
+      <c r="G38" s="55">
         <v>1</v>
       </c>
       <c r="H38" s="11">
@@ -13113,7 +13113,7 @@
       <c r="F39" s="11">
         <v>1</v>
       </c>
-      <c r="G39" s="56">
+      <c r="G39" s="55">
         <v>2</v>
       </c>
       <c r="H39" s="11">
@@ -13151,7 +13151,7 @@
       <c r="F40" s="11">
         <v>0</v>
       </c>
-      <c r="G40" s="56">
+      <c r="G40" s="55">
         <v>3</v>
       </c>
       <c r="H40" s="11">
@@ -13189,7 +13189,7 @@
       <c r="F41" s="11">
         <v>0</v>
       </c>
-      <c r="G41" s="56">
+      <c r="G41" s="55">
         <v>3</v>
       </c>
       <c r="H41" s="11">
@@ -13227,7 +13227,7 @@
       <c r="F42" s="11">
         <v>0</v>
       </c>
-      <c r="G42" s="56">
+      <c r="G42" s="55">
         <v>4</v>
       </c>
       <c r="H42" s="11">
@@ -13265,7 +13265,7 @@
       <c r="F43" s="11">
         <v>0</v>
       </c>
-      <c r="G43" s="56">
+      <c r="G43" s="55">
         <v>5</v>
       </c>
       <c r="H43" s="11">
@@ -13303,7 +13303,7 @@
       <c r="F44" s="11">
         <v>0</v>
       </c>
-      <c r="G44" s="56">
+      <c r="G44" s="55">
         <v>0</v>
       </c>
       <c r="H44" s="11">
@@ -13341,7 +13341,7 @@
       <c r="F45" s="11">
         <v>0</v>
       </c>
-      <c r="G45" s="56">
+      <c r="G45" s="55">
         <v>0</v>
       </c>
       <c r="H45" s="11">
@@ -13379,7 +13379,7 @@
       <c r="F46" s="11">
         <v>1</v>
       </c>
-      <c r="G46" s="56">
+      <c r="G46" s="55">
         <v>1</v>
       </c>
       <c r="H46" s="11">
@@ -13417,7 +13417,7 @@
       <c r="F47" s="11">
         <v>7</v>
       </c>
-      <c r="G47" s="56">
+      <c r="G47" s="55">
         <v>6</v>
       </c>
       <c r="H47" s="11">
@@ -13455,7 +13455,7 @@
       <c r="F48" s="11">
         <v>7</v>
       </c>
-      <c r="G48" s="56">
+      <c r="G48" s="55">
         <v>4</v>
       </c>
       <c r="H48" s="11">
@@ -13493,7 +13493,7 @@
       <c r="F49" s="11">
         <v>6</v>
       </c>
-      <c r="G49" s="56">
+      <c r="G49" s="55">
         <v>4</v>
       </c>
       <c r="H49" s="11">
@@ -13531,7 +13531,7 @@
       <c r="F50" s="11">
         <v>6</v>
       </c>
-      <c r="G50" s="56">
+      <c r="G50" s="55">
         <v>3</v>
       </c>
       <c r="H50" s="11">
@@ -13569,7 +13569,7 @@
       <c r="F51" s="11">
         <v>6</v>
       </c>
-      <c r="G51" s="56">
+      <c r="G51" s="55">
         <v>7</v>
       </c>
       <c r="H51" s="11">
@@ -13607,7 +13607,7 @@
       <c r="F52" s="11">
         <v>6</v>
       </c>
-      <c r="G52" s="56">
+      <c r="G52" s="55">
         <v>0</v>
       </c>
       <c r="H52" s="11">
@@ -13795,9 +13795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54:J64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13872,7 +13872,7 @@
       <c r="F2" s="11">
         <v>0</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="55">
         <v>6</v>
       </c>
       <c r="H2" s="11">
@@ -13910,7 +13910,7 @@
       <c r="F3" s="11">
         <v>0</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="55">
         <v>1</v>
       </c>
       <c r="H3" s="11">
@@ -13948,7 +13948,7 @@
       <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="55">
         <v>2</v>
       </c>
       <c r="H4" s="11">
@@ -13986,7 +13986,7 @@
       <c r="F5" s="11">
         <v>0</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="55">
         <v>3</v>
       </c>
       <c r="H5" s="11">
@@ -14024,7 +14024,7 @@
       <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="55">
         <v>6</v>
       </c>
       <c r="H6" s="11">
@@ -14062,8 +14062,8 @@
       <c r="F7" s="11">
         <v>1</v>
       </c>
-      <c r="G7" s="11">
-        <v>4</v>
+      <c r="G7" s="55">
+        <v>5</v>
       </c>
       <c r="H7" s="11">
         <v>0</v>
@@ -14100,7 +14100,7 @@
       <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="55">
         <v>3</v>
       </c>
       <c r="H8" s="11">
@@ -14138,7 +14138,7 @@
       <c r="F9" s="11">
         <v>0</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="55">
         <v>3</v>
       </c>
       <c r="H9" s="11">
@@ -14176,8 +14176,8 @@
       <c r="F10" s="11">
         <v>0</v>
       </c>
-      <c r="G10" s="11">
-        <v>5</v>
+      <c r="G10" s="55">
+        <v>6</v>
       </c>
       <c r="H10" s="11">
         <v>0</v>
@@ -14214,7 +14214,7 @@
       <c r="F11" s="11">
         <v>1</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="55">
         <v>7</v>
       </c>
       <c r="H11" s="11">
@@ -14252,7 +14252,7 @@
       <c r="F12" s="11">
         <v>0</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="55">
         <v>1</v>
       </c>
       <c r="H12" s="11">
@@ -14290,7 +14290,7 @@
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="55">
         <v>0</v>
       </c>
       <c r="H13" s="11">
@@ -14328,7 +14328,7 @@
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="55">
         <v>2</v>
       </c>
       <c r="H14" s="11">
@@ -14366,7 +14366,7 @@
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="55">
         <v>2</v>
       </c>
       <c r="H15" s="11">
@@ -14404,7 +14404,7 @@
       <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="55">
         <v>1</v>
       </c>
       <c r="H16" s="11">
@@ -14442,8 +14442,8 @@
       <c r="F17" s="11">
         <v>0</v>
       </c>
-      <c r="G17" s="11">
-        <v>7</v>
+      <c r="G17" s="55">
+        <v>10</v>
       </c>
       <c r="H17" s="11">
         <v>0</v>
@@ -14480,7 +14480,7 @@
       <c r="F18" s="11">
         <v>0</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="55">
         <v>1</v>
       </c>
       <c r="H18" s="11">
@@ -14518,7 +14518,7 @@
       <c r="F19" s="11">
         <v>0</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="55">
         <v>4</v>
       </c>
       <c r="H19" s="11">
@@ -14556,7 +14556,7 @@
       <c r="F20" s="11">
         <v>0</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="55">
         <v>1</v>
       </c>
       <c r="H20" s="11">
@@ -14594,7 +14594,7 @@
       <c r="F21" s="11">
         <v>1</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="55">
         <v>4</v>
       </c>
       <c r="H21" s="11">
@@ -14632,8 +14632,8 @@
       <c r="F22" s="11">
         <v>0</v>
       </c>
-      <c r="G22" s="11">
-        <v>5</v>
+      <c r="G22" s="55">
+        <v>7</v>
       </c>
       <c r="H22" s="11">
         <v>0</v>
@@ -14670,7 +14670,7 @@
       <c r="F23" s="11">
         <v>0</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="55">
         <v>1</v>
       </c>
       <c r="H23" s="11">
@@ -14708,8 +14708,8 @@
       <c r="F24" s="11">
         <v>0</v>
       </c>
-      <c r="G24" s="11">
-        <v>1</v>
+      <c r="G24" s="55">
+        <v>2</v>
       </c>
       <c r="H24" s="11">
         <v>0</v>
@@ -14746,7 +14746,7 @@
       <c r="F25" s="11">
         <v>1</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="55">
         <v>4</v>
       </c>
       <c r="H25" s="11">
@@ -14784,7 +14784,7 @@
       <c r="F26" s="11">
         <v>0</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="55">
         <v>3</v>
       </c>
       <c r="H26" s="11">
@@ -14822,7 +14822,7 @@
       <c r="F27" s="11">
         <v>0</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="55">
         <v>1</v>
       </c>
       <c r="H27" s="11">
@@ -14860,7 +14860,7 @@
       <c r="F28" s="11">
         <v>0</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="55">
         <v>6</v>
       </c>
       <c r="H28" s="11">
@@ -14898,7 +14898,7 @@
       <c r="F29" s="11">
         <v>0</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="55">
         <v>3</v>
       </c>
       <c r="H29" s="11">
@@ -14936,7 +14936,7 @@
       <c r="F30" s="11">
         <v>0</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="55">
         <v>2</v>
       </c>
       <c r="H30" s="11">
@@ -14974,7 +14974,7 @@
       <c r="F31" s="11">
         <v>0</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="55">
         <v>2</v>
       </c>
       <c r="H31" s="11">
@@ -15012,8 +15012,8 @@
       <c r="F32" s="11">
         <v>1</v>
       </c>
-      <c r="G32" s="11">
-        <v>8</v>
+      <c r="G32" s="55">
+        <v>9</v>
       </c>
       <c r="H32" s="11">
         <v>0</v>
@@ -15050,7 +15050,7 @@
       <c r="F33" s="11">
         <v>5</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="55">
         <v>2</v>
       </c>
       <c r="H33" s="11">
@@ -15088,7 +15088,7 @@
       <c r="F34" s="11">
         <v>5</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="55">
         <v>2</v>
       </c>
       <c r="H34" s="11">
@@ -15126,7 +15126,7 @@
       <c r="F35" s="11">
         <v>2</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="55">
         <v>1</v>
       </c>
       <c r="H35" s="11">
@@ -15164,7 +15164,7 @@
       <c r="F36" s="11">
         <v>6</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="55">
         <v>0</v>
       </c>
       <c r="H36" s="11">
@@ -15202,7 +15202,7 @@
       <c r="F37" s="11">
         <v>6</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="55">
         <v>7</v>
       </c>
       <c r="H37" s="11">
@@ -15240,7 +15240,7 @@
       <c r="F38" s="11">
         <v>2</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="55">
         <v>4</v>
       </c>
       <c r="H38" s="11">
@@ -15278,7 +15278,7 @@
       <c r="F39" s="11">
         <v>1</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="55">
         <v>1</v>
       </c>
       <c r="H39" s="11">
@@ -15316,7 +15316,7 @@
       <c r="F40" s="11">
         <v>1</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="55">
         <v>4</v>
       </c>
       <c r="H40" s="11">
@@ -15354,7 +15354,7 @@
       <c r="F41" s="11">
         <v>5</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="55">
         <v>2</v>
       </c>
       <c r="H41" s="11">
@@ -15392,7 +15392,7 @@
       <c r="F42" s="11">
         <v>6</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="55">
         <v>9</v>
       </c>
       <c r="H42" s="11">
@@ -15430,7 +15430,7 @@
       <c r="F43" s="11">
         <v>4</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="55">
         <v>2</v>
       </c>
       <c r="H43" s="11">
@@ -15468,7 +15468,7 @@
       <c r="F44" s="11">
         <v>0</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="55">
         <v>9</v>
       </c>
       <c r="H44" s="11">
@@ -15506,7 +15506,7 @@
       <c r="F45" s="11">
         <v>1</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="55">
         <v>8</v>
       </c>
       <c r="H45" s="11">
@@ -15544,7 +15544,7 @@
       <c r="F46" s="11">
         <v>2</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="55">
         <v>0</v>
       </c>
       <c r="H46" s="11">
@@ -15582,8 +15582,8 @@
       <c r="F47" s="11">
         <v>7</v>
       </c>
-      <c r="G47" s="11">
-        <v>2</v>
+      <c r="G47" s="55">
+        <v>3</v>
       </c>
       <c r="H47" s="11">
         <v>0</v>
@@ -15620,7 +15620,7 @@
       <c r="F48" s="11">
         <v>5</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G48" s="55">
         <v>11</v>
       </c>
       <c r="H48" s="11">
@@ -15658,7 +15658,7 @@
       <c r="F49" s="11">
         <v>6</v>
       </c>
-      <c r="G49" s="11">
+      <c r="G49" s="55">
         <v>1</v>
       </c>
       <c r="H49" s="11">
@@ -15696,7 +15696,7 @@
       <c r="F50" s="11">
         <v>4</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="55">
         <v>6</v>
       </c>
       <c r="H50" s="11">
@@ -15734,8 +15734,8 @@
       <c r="F51" s="11">
         <v>6</v>
       </c>
-      <c r="G51" s="11">
-        <v>5</v>
+      <c r="G51" s="55">
+        <v>6</v>
       </c>
       <c r="H51" s="11">
         <v>0</v>
@@ -15772,7 +15772,7 @@
       <c r="F52" s="11">
         <v>9</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="55">
         <v>3</v>
       </c>
       <c r="H52" s="11">
@@ -15817,7 +15817,7 @@
       </c>
       <c r="G53" s="20">
         <f t="shared" si="0"/>
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="H53" s="20">
         <f t="shared" si="0"/>
@@ -15846,7 +15846,7 @@
       </c>
       <c r="F54">
         <f>G53</f>
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="J54">
         <f>B53-C53</f>
@@ -15897,7 +15897,7 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F59">
         <f>SUM(F54:F58)</f>
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="J59">
         <f>SUM(J54:J58)</f>
@@ -15907,7 +15907,7 @@
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F60">
         <f>K53-F59</f>
-        <v>2036</v>
+        <v>2025</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
nmv 27 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 1.1 TO 1.8.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TS 1.1" sheetId="8" r:id="rId1"/>
@@ -4326,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -5837,7 +5837,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -9476,7 +9476,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
@@ -11631,7 +11631,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L53"/>
     </sheetView>
   </sheetViews>
@@ -13795,7 +13795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L53"/>
     </sheetView>
@@ -15949,9 +15949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45:K56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16023,10 +16023,10 @@
       <c r="E2" s="11">
         <v>0</v>
       </c>
-      <c r="F2" s="11">
-        <v>0</v>
-      </c>
-      <c r="G2" s="11">
+      <c r="F2" s="55">
+        <v>0</v>
+      </c>
+      <c r="G2" s="55">
         <v>3</v>
       </c>
       <c r="H2" s="11">
@@ -16061,10 +16061,10 @@
       <c r="E3" s="11">
         <v>0</v>
       </c>
-      <c r="F3" s="11">
-        <v>1</v>
-      </c>
-      <c r="G3" s="11">
+      <c r="F3" s="55">
+        <v>1</v>
+      </c>
+      <c r="G3" s="55">
         <v>0</v>
       </c>
       <c r="H3" s="11">
@@ -16099,10 +16099,10 @@
       <c r="E4" s="11">
         <v>0</v>
       </c>
-      <c r="F4" s="11">
-        <v>1</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="55">
+        <v>1</v>
+      </c>
+      <c r="G4" s="55">
         <v>1</v>
       </c>
       <c r="H4" s="11">
@@ -16137,11 +16137,11 @@
       <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="55">
         <v>9</v>
       </c>
-      <c r="G5" s="11">
-        <v>2</v>
+      <c r="G5" s="55">
+        <v>3</v>
       </c>
       <c r="H5" s="11">
         <v>0</v>
@@ -16175,10 +16175,10 @@
       <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="55">
         <v>3</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="55">
         <v>7</v>
       </c>
       <c r="H6" s="11">
@@ -16213,10 +16213,10 @@
       <c r="E7" s="11">
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="55">
         <v>2</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="55">
         <v>3</v>
       </c>
       <c r="H7" s="11">
@@ -16254,8 +16254,8 @@
       <c r="F8" s="11">
         <v>3</v>
       </c>
-      <c r="G8" s="11">
-        <v>4</v>
+      <c r="G8" s="55">
+        <v>5</v>
       </c>
       <c r="H8" s="11">
         <v>0</v>
@@ -16292,7 +16292,7 @@
       <c r="F9" s="11">
         <v>7</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="55">
         <v>5</v>
       </c>
       <c r="H9" s="11">
@@ -16330,7 +16330,7 @@
       <c r="F10" s="11">
         <v>6</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="55">
         <v>1</v>
       </c>
       <c r="H10" s="11">
@@ -16368,7 +16368,7 @@
       <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="55">
         <v>1</v>
       </c>
       <c r="H11" s="11">
@@ -16406,7 +16406,7 @@
       <c r="F12" s="11">
         <v>6</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="55">
         <v>3</v>
       </c>
       <c r="H12" s="11">
@@ -16444,7 +16444,7 @@
       <c r="F13" s="11">
         <v>0</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="55">
         <v>1</v>
       </c>
       <c r="H13" s="11">
@@ -16482,8 +16482,8 @@
       <c r="F14" s="11">
         <v>1</v>
       </c>
-      <c r="G14" s="11">
-        <v>1</v>
+      <c r="G14" s="55">
+        <v>2</v>
       </c>
       <c r="H14" s="11">
         <v>0</v>
@@ -16520,7 +16520,7 @@
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="55">
         <v>5</v>
       </c>
       <c r="H15" s="11">
@@ -16558,7 +16558,7 @@
       <c r="F16" s="11">
         <v>0</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="55">
         <v>1</v>
       </c>
       <c r="H16" s="11">
@@ -16596,8 +16596,8 @@
       <c r="F17" s="11">
         <v>0</v>
       </c>
-      <c r="G17" s="11">
-        <v>1</v>
+      <c r="G17" s="55">
+        <v>2</v>
       </c>
       <c r="H17" s="11">
         <v>0</v>
@@ -16634,7 +16634,7 @@
       <c r="F18" s="11">
         <v>1</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="55">
         <v>1</v>
       </c>
       <c r="H18" s="11">
@@ -16672,7 +16672,7 @@
       <c r="F19" s="11">
         <v>0</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="55">
         <v>1</v>
       </c>
       <c r="H19" s="11">
@@ -16710,7 +16710,7 @@
       <c r="F20" s="11">
         <v>1</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="55">
         <v>3</v>
       </c>
       <c r="H20" s="11">
@@ -16748,7 +16748,7 @@
       <c r="F21" s="11">
         <v>3</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="55">
         <v>1</v>
       </c>
       <c r="H21" s="11">
@@ -16786,7 +16786,7 @@
       <c r="F22" s="11">
         <v>2</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="55">
         <v>2</v>
       </c>
       <c r="H22" s="11">
@@ -16824,7 +16824,7 @@
       <c r="F23" s="11">
         <v>1</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="55">
         <v>0</v>
       </c>
       <c r="H23" s="11">
@@ -16862,7 +16862,7 @@
       <c r="F24" s="11">
         <v>1</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="55">
         <v>1</v>
       </c>
       <c r="H24" s="11">
@@ -16900,7 +16900,7 @@
       <c r="F25" s="11">
         <v>0</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="55">
         <v>4</v>
       </c>
       <c r="H25" s="11">
@@ -16938,7 +16938,7 @@
       <c r="F26" s="11">
         <v>1</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="55">
         <v>1</v>
       </c>
       <c r="H26" s="11">
@@ -16976,7 +16976,7 @@
       <c r="F27" s="11">
         <v>2</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="55">
         <v>0</v>
       </c>
       <c r="H27" s="11">
@@ -17014,7 +17014,7 @@
       <c r="F28" s="11">
         <v>2</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="55">
         <v>1</v>
       </c>
       <c r="H28" s="11">
@@ -17052,7 +17052,7 @@
       <c r="F29" s="11">
         <v>4</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="55">
         <v>3</v>
       </c>
       <c r="H29" s="11">
@@ -17090,7 +17090,7 @@
       <c r="F30" s="11">
         <v>0</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="55">
         <v>1</v>
       </c>
       <c r="H30" s="11">
@@ -17128,7 +17128,7 @@
       <c r="F31" s="11">
         <v>2</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="55">
         <v>0</v>
       </c>
       <c r="H31" s="11">
@@ -17166,7 +17166,7 @@
       <c r="F32" s="11">
         <v>0</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="55">
         <v>5</v>
       </c>
       <c r="H32" s="11">
@@ -17204,7 +17204,7 @@
       <c r="F33" s="11">
         <v>2</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="55">
         <v>1</v>
       </c>
       <c r="H33" s="11">
@@ -17242,7 +17242,7 @@
       <c r="F34" s="11">
         <v>1</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="55">
         <v>1</v>
       </c>
       <c r="H34" s="11">
@@ -17280,7 +17280,7 @@
       <c r="F35" s="11">
         <v>1</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="55">
         <v>1</v>
       </c>
       <c r="H35" s="11">
@@ -17318,7 +17318,7 @@
       <c r="F36" s="11">
         <v>1</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="55">
         <v>3</v>
       </c>
       <c r="H36" s="11">
@@ -17356,7 +17356,7 @@
       <c r="F37" s="11">
         <v>1</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="55">
         <v>2</v>
       </c>
       <c r="H37" s="11">
@@ -17394,7 +17394,7 @@
       <c r="F38" s="11">
         <v>7</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="55">
         <v>3</v>
       </c>
       <c r="H38" s="11">
@@ -17432,7 +17432,7 @@
       <c r="F39" s="11">
         <v>6</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="55">
         <v>6</v>
       </c>
       <c r="H39" s="11">
@@ -17470,7 +17470,7 @@
       <c r="F40" s="11">
         <v>7</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="55">
         <v>2</v>
       </c>
       <c r="H40" s="11">
@@ -17508,7 +17508,7 @@
       <c r="F41" s="11">
         <v>7</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="55">
         <v>4</v>
       </c>
       <c r="H41" s="11">
@@ -17546,7 +17546,7 @@
       <c r="F42" s="11">
         <v>6</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="55">
         <v>3</v>
       </c>
       <c r="H42" s="11">
@@ -17584,7 +17584,7 @@
       <c r="F43" s="11">
         <v>9</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="55">
         <v>4</v>
       </c>
       <c r="H43" s="11">
@@ -17629,7 +17629,7 @@
       </c>
       <c r="G44" s="13">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H44" s="13">
         <f t="shared" si="0"/>
@@ -17662,7 +17662,7 @@
       </c>
       <c r="F45">
         <f>G44</f>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="J45">
         <f>B44-C44</f>
@@ -17715,7 +17715,7 @@
     <row r="50" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F50">
         <f>SUM(F45:F49)</f>
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="J50">
         <f>SUM(J45:J49)</f>
@@ -17725,7 +17725,7 @@
     <row r="51" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F51">
         <f>K44-F50</f>
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>102</v>
@@ -17765,10 +17765,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17865,32 +17865,32 @@
         <v>305</v>
       </c>
       <c r="E3" s="32">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="F3" s="32">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="G3" s="32">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="H3" s="32">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="I3" s="32">
-        <v>2139</v>
+        <v>2129</v>
       </c>
       <c r="J3" s="32">
-        <v>1966</v>
+        <v>1941</v>
       </c>
       <c r="K3" s="32">
-        <v>2036</v>
+        <v>2025</v>
       </c>
       <c r="L3" s="32">
-        <v>1622</v>
+        <v>1618</v>
       </c>
       <c r="M3" s="32">
         <f>SUM(E3:L3)</f>
-        <v>12923</v>
+        <v>12862</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="34.5" x14ac:dyDescent="0.25">
@@ -17904,32 +17904,32 @@
         <v>307</v>
       </c>
       <c r="E4" s="32">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F4" s="32">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G4" s="32">
+        <v>99</v>
+      </c>
+      <c r="H4" s="32">
+        <v>92</v>
+      </c>
+      <c r="I4" s="32">
+        <v>191</v>
+      </c>
+      <c r="J4" s="32">
+        <v>144</v>
+      </c>
+      <c r="K4" s="32">
+        <v>189</v>
+      </c>
+      <c r="L4" s="32">
         <v>97</v>
-      </c>
-      <c r="H4" s="32">
-        <v>87</v>
-      </c>
-      <c r="I4" s="32">
-        <v>181</v>
-      </c>
-      <c r="J4" s="32">
-        <v>119</v>
-      </c>
-      <c r="K4" s="32">
-        <v>178</v>
-      </c>
-      <c r="L4" s="32">
-        <v>93</v>
       </c>
       <c r="M4" s="32">
         <f t="shared" ref="M4:M7" si="0">SUM(E4:L4)</f>
-        <v>981</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="69" x14ac:dyDescent="0.25">
@@ -18092,9 +18092,6 @@
         <v>16572</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>